<commit_message>
feat(ExportToExcel): add core exporter feature with excel template
</commit_message>
<xml_diff>
--- a/src/assets/template.xlsx
+++ b/src/assets/template.xlsx
@@ -4,12 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Conversations" sheetId="2" r:id="rId2"/>
+    <sheet name="SURA" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Conversations!$A$1:$I$1</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -20,19 +24,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>This is a test</t>
-  </si>
-  <si>
-    <t>D</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>This is a test - summary stuff here…</t>
+  </si>
+  <si>
+    <t>Message Lines</t>
+  </si>
+  <si>
+    <t>assessmentId</t>
+  </si>
+  <si>
+    <t>createdBy</t>
+  </si>
+  <si>
+    <t>conversationId</t>
+  </si>
+  <si>
+    <t>eventKey</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>mcsRawScore</t>
+  </si>
+  <si>
+    <t>agentId</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -52,6 +83,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,20 +118,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,11 +468,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
@@ -446,8 +492,11 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2">
-        <f>COUNTA(Data!A:A)</f>
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>COUNTA(Conversations!A:A)</f>
         <v>1</v>
       </c>
     </row>
@@ -467,20 +516,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>1</v>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
feat(ExporterEffects): complete export of assessments grid
</commit_message>
<xml_diff>
--- a/src/assets/template.xlsx
+++ b/src/assets/template.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Conversations" sheetId="2" r:id="rId2"/>
-    <sheet name="SURA" sheetId="3" r:id="rId3"/>
+    <sheet name="Assessments" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Conversations!$A$1:$I$1</definedName>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>This is a test - summary stuff here…</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>note</t>
+  </si>
+  <si>
+    <t>Assessments</t>
   </si>
 </sst>
 </file>
@@ -127,10 +130,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -466,30 +469,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
@@ -498,6 +501,15 @@
       <c r="B2">
         <f>COUNTA(Conversations!A:A)</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <f>COUNTA(Assessments!A:A)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -518,38 +530,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -568,7 +580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>